<commit_message>
Some corrections, Java upgrade to 8u60, libraries JETT/Tika/Hibernate validator upgrades.
</commit_message>
<xml_diff>
--- a/RETA-core/src/main/java/com/ben12/reta/resources/template/template.xlsx
+++ b/RETA-core/src/main/java/com/ben12/reta/resources/template/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12150" windowHeight="12930"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12150" windowHeight="12930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DOCUMENT" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
     <t>&lt;jt:forEach items="${source.requirements}" var="req"&gt;&lt;jt:if test="${req.getReferencesFor(coverSource).isEmpty() == false}" elseAction="shiftUp"&gt;${req.text}</t>
   </si>
   <si>
-    <t>${jagg:eval(req.getReferencesFor(coverSource), 'com.ben12.reta.util.ConcatAggregator(text, "'+line+'")')}&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>${source.sourcePath}</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>&lt;jt:forEach items="${source.requirements}" var="req"&gt;&lt;jt:if test="${req.getReferredByRequirementFor(coverBySource).isEmpty() == false}" elseAction="shiftUp"&gt;${req.text}</t>
   </si>
   <si>
-    <t>${jagg:eval(req.getReferredByRequirementFor(coverBySource), 'com.ben12.reta.util.ConcatAggregator(text, "'+line+'")')}&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>&lt;jt:span factor="${attributes.size()+1}" expandRight="true" value="${source.sourcePath}" /&gt;</t>
   </si>
   <si>
@@ -89,16 +83,22 @@
     <t>&lt;jt:if test="${!req.referredBySource.isEmpty() &amp;&amp; req.referredBySource.size()&lt;source.coversBy.size()}" elseAction="shiftUp"&gt;${req.getAttribute(attribute)}&lt;/jt:if&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:if test="${!req.referredBySource.isEmpty() &amp;&amp; req.referredBySource.size()&lt;source.coversBy.size()}" elseAction="shiftUp"&gt;${jagg:eval(req.referredBySource, 'com.ben12.reta.util.ConcatAggregator(name, "'+line+'")')}&lt;/jt:if&gt;</t>
-  </si>
-  <si>
-    <t>&lt;jt:if test="${req.referredBySource.size()&gt;=source.coversBy.size()}" elseAction="shiftUp"&gt;${jagg:eval(req.referredBySource, 'com.ben12.reta.util.ConcatAggregator(name, "'+line+'")')}&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>&lt;jt:forEach items="${source.requirements}" var="req"&gt;&lt;jt:if test="${req.referredBySource.isEmpty() &amp;&amp; !source.coversBy.isEmpty()}" elseAction="shiftUp"&gt;${req.getAttribute(attribute)}&lt;/jt:if&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:forEach items="${source.requirements}" var="req"&gt;&lt;jt:if test="${req.referredBySource.isEmpty() &amp;&amp; !source.coversBy.isEmpty()}" elseAction="shiftUp"&gt;${jagg:eval(req.referredBySource, 'com.ben12.reta.util.ConcatAggregator(name, "'+line+'")')}&lt;/jt:if&gt;</t>
+    <t>&lt;jt:forEach items="${source.requirements}" var="req"&gt;&lt;jt:if test="${req.referredBySource.isEmpty() &amp;&amp; !source.coversBy.isEmpty()}" elseAction="shiftUp"&gt;${jagg:eval(req.referredBySource, 'Concat(name, "'+line+'")')}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${!req.referredBySource.isEmpty() &amp;&amp; req.referredBySource.size()&lt;source.coversBy.size()}" elseAction="shiftUp"&gt;${jagg:eval(req.referredBySource, 'Concat(name, "'+line+'")')}&lt;/jt:if&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:if test="${req.referredBySource.size()&gt;=source.coversBy.size()}" elseAction="shiftUp"&gt;${jagg:eval(req.referredBySource, 'Concat(name, "'+line+'")')}&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${jagg:eval(req.getReferencesFor(coverSource), 'Concat(text, "'+line+'")')}&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
+  </si>
+  <si>
+    <t>${jagg:eval(req.getReferredByRequirementFor(coverBySource), 'Concat(text, "'+line+'")')}&lt;/jt:if&gt;&lt;/jt:forEach&gt;</t>
   </si>
 </sst>
 </file>
@@ -106,8 +106,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="172" formatCode="\R\e\q\u\i\r\e\m\e\n\t\ \c\o\u\n\t\:\ ###,##0"/>
-    <numFmt numFmtId="176" formatCode="\U\n\k\o\w\n\ \r\e\f\e\r\e\n\c\e\ \c\o\u\n\t\:\ ###,##0"/>
+    <numFmt numFmtId="164" formatCode="\R\e\q\u\i\r\e\m\e\n\t\ \c\o\u\n\t\:\ ###,##0"/>
+    <numFmt numFmtId="165" formatCode="\U\n\k\o\w\n\ \r\e\f\e\r\e\n\c\e\ \c\o\u\n\t\:\ ###,##0"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -256,7 +256,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,24 +277,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="172" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -304,10 +294,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -316,6 +306,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,8 +616,8 @@
   </sheetPr>
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="52.5703125" defaultRowHeight="12.75"/>
@@ -628,7 +628,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="8" customFormat="1">
       <c r="A1" s="13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -638,8 +638,8 @@
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" s="8" customFormat="1">
-      <c r="A2" s="18" t="s">
-        <v>13</v>
+      <c r="A2" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -650,7 +650,7 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -666,29 +666,29 @@
       <c r="F5" s="6"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="76.5">
-      <c r="A6" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>27</v>
+    <row r="6" spans="1:7" ht="63.75">
+      <c r="A6" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="63.75">
-      <c r="A7" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="28" t="s">
+    <row r="7" spans="1:7" ht="51">
+      <c r="A7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="63.75">
-      <c r="A8" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="29" t="s">
+      <c r="A8" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -722,28 +722,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="20"/>
+      <c r="A2" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="28"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="15"/>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
     </row>
@@ -752,74 +752,74 @@
         <v>6</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="15"/>
+      <c r="A8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="26"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>9</v>
+      <c r="B9" s="16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="38.25">
       <c r="A10" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="16"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="26"/>
-      <c r="D13" s="16"/>
+      <c r="A13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="22"/>
+      <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="22" t="s">
+      <c r="A14" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="29"/>
+      <c r="B15" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="51">
+      <c r="A16" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="51">
-      <c r="A16" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="17" spans="2:2">
-      <c r="B17" s="16"/>
+      <c r="B17" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>